<commit_message>
remove logic convertors for SPI
</commit_message>
<xml_diff>
--- a/BOM/BOM[mod_duo_x_g3399].xlsx
+++ b/BOM/BOM[mod_duo_x_g3399].xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Clients\MOD Devices GmbH\MOD DUO X-CB-G3399\20191013\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Clients\MOD Devices GmbH\MOD DUO X-CB-G3399\20191018\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Designator</t>
   </si>
@@ -206,21 +206,6 @@
     <t>H11706CT-ND</t>
   </si>
   <si>
-    <t>Q1, Q2, Q3</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 60V 115MA SOT-23</t>
-  </si>
-  <si>
-    <t>ON Semiconductor / Fairchild</t>
-  </si>
-  <si>
-    <t>2N7002</t>
-  </si>
-  <si>
-    <t>2N7002NCT-ND</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -243,45 +228,6 @@
   </si>
   <si>
     <t>311-100KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R6, R7, R8, R9, R10, R11</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>RES SMD 3.9K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>Stackpole Electronics</t>
-  </si>
-  <si>
-    <t>RMCF0402FT3K90</t>
-  </si>
-  <si>
-    <t>RMCF0402FT3K90CT-ND</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>RES 8.2K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RMCF0402FT8K20</t>
-  </si>
-  <si>
-    <t>RMCF0402FT8K20CT-ND</t>
   </si>
   <si>
     <t>U1</t>
@@ -646,18 +592,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -986,38 +932,38 @@
         <v>61</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
         <v>15</v>
@@ -1036,7 +982,7 @@
         <v>69</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>70</v>
@@ -1063,128 +1009,20 @@
         <v>74</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="69" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="70" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>